<commit_message>
update weekly scrum(this needs to be converted to sprint backlog)
</commit_message>
<xml_diff>
--- a/documents/Extra/Weekly Scrum.xlsx
+++ b/documents/Extra/Weekly Scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KoreixX\Documents\GitHub\Software2project\documents\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cadew\OneDrive\Documents\GitHub\Software2project\documents\Extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Meeting #</t>
   </si>
@@ -125,6 +125,18 @@
   </si>
   <si>
     <t>B, X</t>
+  </si>
+  <si>
+    <t>Backened - search for and properly set up python for mysql</t>
+  </si>
+  <si>
+    <t>Backened - search for and properly set up python for mysql/begin averaging calculations</t>
+  </si>
+  <si>
+    <t>backend - translate python into java due to database errors caused in python parsing</t>
+  </si>
+  <si>
+    <t>w</t>
   </si>
 </sst>
 </file>
@@ -482,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1000"/>
+  <dimension ref="A1:H1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -617,69 +629,100 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>6</v>
-      </c>
+      <c r="A7" s="3"/>
       <c r="B7" s="4">
-        <v>43154</v>
+        <v>43151</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
+      <c r="A8" s="3"/>
       <c r="B8" s="4">
-        <v>43157</v>
+        <v>43153</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>25</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="4">
         <v>43154</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="4">
         <v>43157</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4">
+        <v>43154</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4">
+        <v>43157</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
-    </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="4">
+        <v>43157</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
@@ -729,10 +772,10 @@
     <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
     </row>
-    <row r="30" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="4"/>
     </row>
     <row r="32" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
@@ -3641,6 +3684,12 @@
     </row>
     <row r="1000" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B1000" s="4"/>
+    </row>
+    <row r="1001" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1001" s="4"/>
+    </row>
+    <row r="1002" spans="2:2" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B1002" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>